<commit_message>
Change Python Code and PrefaultVoltage Tab
</commit_message>
<xml_diff>
--- a/Foward Backward LoadFlow Solver/data.xlsx
+++ b/Foward Backward LoadFlow Solver/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\load-flow-solver-ui-master\Foward Backward LoadFlow Solver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\load-flow-solver-ui-master\Foward Backward LoadFlow Solver\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AC2355-8A40-4921-84C1-92EF6A239AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7531EDF5-7D52-4C93-A082-FBDA00E267AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="4200" windowWidth="21600" windowHeight="12855" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="21600" windowHeight="12855" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="edges" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,14 @@
     <sheet name="fbsweep" sheetId="5" r:id="rId5"/>
     <sheet name="finaldata" sheetId="6" r:id="rId6"/>
     <sheet name="linesequ" sheetId="7" r:id="rId7"/>
+    <sheet name="prefaultvoltages" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Start Node</t>
   </si>
@@ -89,6 +90,27 @@
   </si>
   <si>
     <t>Imeg Part</t>
+  </si>
+  <si>
+    <t>Bus</t>
+  </si>
+  <si>
+    <t>PhaseA(Re)</t>
+  </si>
+  <si>
+    <t>PhaseA(Im)</t>
+  </si>
+  <si>
+    <t>PhaseB(Re)</t>
+  </si>
+  <si>
+    <t>PhaseB(Im)</t>
+  </si>
+  <si>
+    <t>PhaseC(Re)</t>
+  </si>
+  <si>
+    <t>PhaseC(Im)</t>
   </si>
 </sst>
 </file>
@@ -645,7 +667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A16AFA0-F1F5-4C37-98A0-A9E08CB2EE28}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -674,4 +696,42 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC3167AD-089A-4A26-93CE-E22ACB28DC04}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>